<commit_message>
Added Cochez as a Work Payment
</commit_message>
<xml_diff>
--- a/files/all_credit_card.xlsx
+++ b/files/all_credit_card.xlsx
@@ -660,9 +660,9 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L77"/>
+  <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -748,7 +748,7 @@
     <row r="9" ht="30.1" customHeight="1">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B9" s="15" t="inlineStr">
@@ -758,13 +758,13 @@
       </c>
       <c r="C9" s="5" t="inlineStr"/>
       <c r="D9" s="6" t="n">
-        <v>5000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="10" ht="30.1" customHeight="1">
       <c r="A10" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>22/04/2021</t>
         </is>
       </c>
       <c r="B10" s="15" t="inlineStr">
@@ -774,13 +774,13 @@
       </c>
       <c r="C10" s="5" t="inlineStr"/>
       <c r="D10" s="6" t="n">
-        <v>2099.16</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="11" ht="30.1" customHeight="1">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B11" s="15" t="inlineStr">
@@ -790,13 +790,13 @@
       </c>
       <c r="C11" s="5" t="inlineStr"/>
       <c r="D11" s="6" t="n">
-        <v>2000</v>
+        <v>2099.16</v>
       </c>
     </row>
     <row r="12" ht="30.1" customHeight="1">
       <c r="A12" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>07/05/2021</t>
         </is>
       </c>
       <c r="B12" s="15" t="inlineStr">
@@ -806,902 +806,902 @@
       </c>
       <c r="C12" s="5" t="inlineStr"/>
       <c r="D12" s="6" t="n">
-        <v>3500</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="13" ht="30.1" customHeight="1">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>15/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B13" s="15" t="inlineStr">
         <is>
-          <t>ESTACION MISTI         PANAMA OESTE  PA</t>
+          <t>SEGURO FRAUDE MENSUAL</t>
         </is>
       </c>
       <c r="C13" s="7" t="n">
-        <v>-27</v>
+        <v>-3.5</v>
       </c>
       <c r="D13" s="6" t="inlineStr"/>
     </row>
     <row r="14" ht="30.1" customHeight="1">
       <c r="A14" s="4" t="inlineStr">
         <is>
-          <t>15/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B14" s="15" t="inlineStr">
         <is>
-          <t>DELICIAS DEL MAR REST  RIO HATO      PA</t>
+          <t>SEGURO DE DESGRAVAMEN</t>
         </is>
       </c>
       <c r="C14" s="7" t="n">
-        <v>-93.3</v>
+        <v>-26.31</v>
       </c>
       <c r="D14" s="6" t="inlineStr"/>
     </row>
     <row r="15" ht="30.1" customHeight="1">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B15" s="15" t="inlineStr">
         <is>
-          <t>ESA FLACA RICA</t>
+          <t>ITBMS CARGO POR SEGURO</t>
         </is>
       </c>
       <c r="C15" s="7" t="n">
-        <v>-15.78</v>
+        <v>-0.18</v>
       </c>
       <c r="D15" s="6" t="inlineStr"/>
     </row>
     <row r="16" ht="30.1" customHeight="1">
       <c r="A16" s="4" t="inlineStr">
         <is>
-          <t>13/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B16" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>ITBMS CARGO POR SEGURO</t>
         </is>
       </c>
       <c r="C16" s="7" t="n">
-        <v>-234.99</v>
+        <v>-1.32</v>
       </c>
       <c r="D16" s="6" t="inlineStr"/>
     </row>
     <row r="17" ht="30.1" customHeight="1">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B17" s="15" t="inlineStr">
         <is>
-          <t>VIAJEMOS.COM           7862359135    FL</t>
+          <t>DELI CLUB</t>
         </is>
       </c>
       <c r="C17" s="7" t="n">
-        <v>-991.15</v>
+        <v>-11.7</v>
       </c>
       <c r="D17" s="6" t="inlineStr"/>
     </row>
     <row r="18" ht="30.1" customHeight="1">
       <c r="A18" s="4" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>17/05/2021</t>
         </is>
       </c>
       <c r="B18" s="15" t="inlineStr">
         <is>
-          <t>FARMACIA ARROCHA ARRAI PANAMA        PA</t>
+          <t>CROCS COSTA VERDE      PANAMA        PA</t>
         </is>
       </c>
       <c r="C18" s="7" t="n">
-        <v>-49.65</v>
+        <v>-29.95</v>
       </c>
       <c r="D18" s="6" t="inlineStr"/>
     </row>
     <row r="19" ht="30.1" customHeight="1">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>11/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B19" s="15" t="inlineStr">
         <is>
-          <t>ESTACION MISTI         PANAMA OESTE  PA</t>
+          <t>PAYPAL *FLOWERSCAIN    4029357733    ON</t>
         </is>
       </c>
       <c r="C19" s="7" t="n">
-        <v>-37</v>
+        <v>-87.90000000000001</v>
       </c>
       <c r="D19" s="6" t="inlineStr"/>
     </row>
     <row r="20" ht="30.1" customHeight="1">
       <c r="A20" s="4" t="inlineStr">
         <is>
-          <t>10/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B20" s="15" t="inlineStr">
         <is>
-          <t>RESTAURANTE LUNG FUNG</t>
+          <t>UBER   *EATS           HELP.UBER.COM ON</t>
         </is>
       </c>
       <c r="C20" s="7" t="n">
-        <v>-59.71</v>
+        <v>-2.34</v>
       </c>
       <c r="D20" s="6" t="inlineStr"/>
     </row>
     <row r="21" ht="30.1" customHeight="1">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B21" s="15" t="inlineStr">
         <is>
-          <t>AMZN Mktp CA*2L8WI6VO1 WWW.AMAZON.CA ON</t>
+          <t>UBER   *EATS           HELP.UBER.COM ON</t>
         </is>
       </c>
       <c r="C21" s="7" t="n">
-        <v>-83.38</v>
+        <v>-23.37</v>
       </c>
       <c r="D21" s="6" t="inlineStr"/>
     </row>
     <row r="22" ht="30.1" customHeight="1">
       <c r="A22" s="4" t="inlineStr">
         <is>
-          <t>08/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B22" s="15" t="inlineStr">
         <is>
-          <t>FARMACIA NUEVO CHORRIL CERRO SILVEST PA</t>
+          <t>RIBA SMITH MARKET PLAZ PUERTO CAIMIT PA</t>
         </is>
       </c>
       <c r="C22" s="7" t="n">
-        <v>-33.3</v>
+        <v>-14.75</v>
       </c>
       <c r="D22" s="6" t="inlineStr"/>
     </row>
     <row r="23" ht="30.1" customHeight="1">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>19/04/2021</t>
         </is>
       </c>
       <c r="B23" s="15" t="inlineStr">
         <is>
-          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+          <t>GONG CHA               PANAMA OESTE  PA</t>
         </is>
       </c>
       <c r="C23" s="7" t="n">
-        <v>-206.98</v>
+        <v>-28.65</v>
       </c>
       <c r="D23" s="6" t="inlineStr"/>
     </row>
     <row r="24" ht="30.1" customHeight="1">
       <c r="A24" s="4" t="inlineStr">
         <is>
-          <t>07/05/2021</t>
+          <t>20/04/2021</t>
         </is>
       </c>
       <c r="B24" s="15" t="inlineStr">
         <is>
-          <t>FARMACIA ARROCHA WESTL PANAMA        PA</t>
+          <t>NETFLIX.COM            866-579-7172  CA</t>
         </is>
       </c>
       <c r="C24" s="7" t="n">
-        <v>-42.04</v>
+        <v>-15.99</v>
       </c>
       <c r="D24" s="6" t="inlineStr"/>
     </row>
     <row r="25" ht="30.1" customHeight="1">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>06/05/2021</t>
+          <t>22/04/2021</t>
         </is>
       </c>
       <c r="B25" s="15" t="inlineStr">
         <is>
-          <t>NOVEY VISTA ALEGRE     PANAMA        PA</t>
+          <t>FELIPE MOTTA</t>
         </is>
       </c>
       <c r="C25" s="7" t="n">
-        <v>-52.42</v>
+        <v>-150.83</v>
       </c>
       <c r="D25" s="6" t="inlineStr"/>
     </row>
     <row r="26" ht="30.1" customHeight="1">
       <c r="A26" s="4" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>22/04/2021</t>
         </is>
       </c>
       <c r="B26" s="15" t="inlineStr">
         <is>
-          <t>Disney Plus            507-8389374   CA</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C26" s="7" t="n">
-        <v>-5.99</v>
+        <v>-74.7</v>
       </c>
       <c r="D26" s="6" t="inlineStr"/>
     </row>
     <row r="27" ht="30.1" customHeight="1">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>24/04/2021</t>
         </is>
       </c>
       <c r="B27" s="15" t="inlineStr">
         <is>
-          <t>Amazon web services    aws.amazon.co WA</t>
+          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
         </is>
       </c>
       <c r="C27" s="7" t="n">
-        <v>-33.21</v>
+        <v>-74.34</v>
       </c>
       <c r="D27" s="6" t="inlineStr"/>
     </row>
     <row r="28" ht="30.1" customHeight="1">
       <c r="A28" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>24/04/2021</t>
         </is>
       </c>
       <c r="B28" s="15" t="inlineStr">
         <is>
-          <t>SPIRIT AINES           MIRAMAR       FL</t>
-        </is>
-      </c>
-      <c r="C28" s="5" t="inlineStr"/>
-      <c r="D28" s="6" t="n">
-        <v>217.07</v>
-      </c>
+          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+        </is>
+      </c>
+      <c r="C28" s="7" t="n">
+        <v>-121.9</v>
+      </c>
+      <c r="D28" s="6" t="inlineStr"/>
     </row>
     <row r="29" ht="30.1" customHeight="1">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>24/04/2021</t>
         </is>
       </c>
       <c r="B29" s="15" t="inlineStr">
         <is>
-          <t>EDREAMS                BARCELONA     ES</t>
+          <t>CLINICA DENTAL AMERICA PANAMA        PA</t>
         </is>
       </c>
       <c r="C29" s="7" t="n">
-        <v>-250.78</v>
+        <v>-130</v>
       </c>
       <c r="D29" s="6" t="inlineStr"/>
     </row>
     <row r="30" ht="30.1" customHeight="1">
       <c r="A30" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>26/04/2021</t>
         </is>
       </c>
       <c r="B30" s="15" t="inlineStr">
         <is>
-          <t>ETT*s269ac1RENT        801-8775491   IL</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C30" s="7" t="n">
-        <v>-369.2</v>
+        <v>-158.99</v>
       </c>
       <c r="D30" s="6" t="inlineStr"/>
     </row>
     <row r="31" ht="30.1" customHeight="1">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>27/04/2021</t>
         </is>
       </c>
       <c r="B31" s="15" t="inlineStr">
         <is>
-          <t>ANTI BURGUER           831-7937      PA</t>
+          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
         </is>
       </c>
       <c r="C31" s="7" t="n">
-        <v>-12</v>
+        <v>-14.54</v>
       </c>
       <c r="D31" s="6" t="inlineStr"/>
     </row>
     <row r="32" ht="30.1" customHeight="1">
       <c r="A32" s="4" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>27/04/2021</t>
         </is>
       </c>
       <c r="B32" s="15" t="inlineStr">
         <is>
-          <t>DELTA</t>
+          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
         </is>
       </c>
       <c r="C32" s="7" t="n">
-        <v>-37</v>
+        <v>-15.1</v>
       </c>
       <c r="D32" s="6" t="inlineStr"/>
     </row>
     <row r="33" ht="30.1" customHeight="1">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>28/04/2021</t>
         </is>
       </c>
       <c r="B33" s="15" t="inlineStr">
         <is>
-          <t>SPIRIT AI4870264393891 MIRAMAR       FL</t>
+          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
         </is>
       </c>
       <c r="C33" s="7" t="n">
-        <v>-217.07</v>
+        <v>-21.97</v>
       </c>
       <c r="D33" s="6" t="inlineStr"/>
     </row>
     <row r="34" ht="30.1" customHeight="1">
       <c r="A34" s="4" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>27/04/2021</t>
         </is>
       </c>
       <c r="B34" s="15" t="inlineStr">
         <is>
-          <t>FELIPE MOTTA</t>
+          <t>CLINICA DENTAL AMERICA</t>
         </is>
       </c>
       <c r="C34" s="7" t="n">
-        <v>-733.72</v>
+        <v>-60</v>
       </c>
       <c r="D34" s="6" t="inlineStr"/>
     </row>
     <row r="35" ht="30.1" customHeight="1">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>03/05/2021</t>
+          <t>29/04/2021</t>
         </is>
       </c>
       <c r="B35" s="15" t="inlineStr">
         <is>
-          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+          <t>MCDONALDS MILLA 8/CUMB PANAMA        PA</t>
         </is>
       </c>
       <c r="C35" s="7" t="n">
-        <v>-261.36</v>
+        <v>-1.5</v>
       </c>
       <c r="D35" s="6" t="inlineStr"/>
     </row>
     <row r="36" ht="30.1" customHeight="1">
       <c r="A36" s="4" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>28/04/2021</t>
         </is>
       </c>
       <c r="B36" s="15" t="inlineStr">
         <is>
-          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+          <t>CLINICA OSPINO</t>
         </is>
       </c>
       <c r="C36" s="7" t="n">
-        <v>-367.96</v>
+        <v>-70</v>
       </c>
       <c r="D36" s="6" t="inlineStr"/>
     </row>
     <row r="37" ht="30.1" customHeight="1">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>30/04/2021</t>
+          <t>29/04/2021</t>
         </is>
       </c>
       <c r="B37" s="15" t="inlineStr">
         <is>
-          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
+          <t>FELIPE MOTTA</t>
         </is>
       </c>
       <c r="C37" s="7" t="n">
-        <v>-476.26</v>
+        <v>-733.72</v>
       </c>
       <c r="D37" s="6" t="inlineStr"/>
     </row>
     <row r="38" ht="30.1" customHeight="1">
       <c r="A38" s="4" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B38" s="15" t="inlineStr">
         <is>
-          <t>CLINICA OSPINO</t>
+          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
         </is>
       </c>
       <c r="C38" s="7" t="n">
-        <v>-70</v>
+        <v>-261.36</v>
       </c>
       <c r="D38" s="6" t="inlineStr"/>
     </row>
     <row r="39" ht="30.1" customHeight="1">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>30/04/2021</t>
         </is>
       </c>
       <c r="B39" s="15" t="inlineStr">
         <is>
-          <t>CLINICA DENTAL AMERICA</t>
+          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
         </is>
       </c>
       <c r="C39" s="7" t="n">
-        <v>-60</v>
+        <v>-367.96</v>
       </c>
       <c r="D39" s="6" t="inlineStr"/>
     </row>
     <row r="40" ht="30.1" customHeight="1">
       <c r="A40" s="4" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>30/04/2021</t>
         </is>
       </c>
       <c r="B40" s="15" t="inlineStr">
         <is>
-          <t>MCDONALDS MILLA 8/CUMB PANAMA        PA</t>
+          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
         </is>
       </c>
       <c r="C40" s="7" t="n">
-        <v>-1.5</v>
+        <v>-476.26</v>
       </c>
       <c r="D40" s="6" t="inlineStr"/>
     </row>
     <row r="41" ht="30.1" customHeight="1">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>30/04/2021</t>
         </is>
       </c>
       <c r="B41" s="15" t="inlineStr">
         <is>
-          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
+          <t>DELTA</t>
         </is>
       </c>
       <c r="C41" s="7" t="n">
-        <v>-14.54</v>
+        <v>-37</v>
       </c>
       <c r="D41" s="6" t="inlineStr"/>
     </row>
     <row r="42" ht="30.1" customHeight="1">
       <c r="A42" s="4" t="inlineStr">
         <is>
-          <t>27/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B42" s="15" t="inlineStr">
         <is>
-          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
+          <t>SPIRIT AI4870264393891 MIRAMAR       FL</t>
         </is>
       </c>
       <c r="C42" s="7" t="n">
-        <v>-15.1</v>
+        <v>-217.07</v>
       </c>
       <c r="D42" s="6" t="inlineStr"/>
     </row>
     <row r="43" ht="30.1" customHeight="1">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B43" s="15" t="inlineStr">
         <is>
-          <t>SUPERMERCADO SUPER CAR PANAMA        PA</t>
-        </is>
-      </c>
-      <c r="C43" s="7" t="n">
-        <v>-21.97</v>
-      </c>
-      <c r="D43" s="6" t="inlineStr"/>
+          <t>SPIRIT AINES           MIRAMAR       FL</t>
+        </is>
+      </c>
+      <c r="C43" s="5" t="inlineStr"/>
+      <c r="D43" s="6" t="n">
+        <v>217.07</v>
+      </c>
     </row>
     <row r="44" ht="30.1" customHeight="1">
       <c r="A44" s="4" t="inlineStr">
         <is>
-          <t>26/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B44" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>EDREAMS                BARCELONA     ES</t>
         </is>
       </c>
       <c r="C44" s="7" t="n">
-        <v>-158.99</v>
+        <v>-250.78</v>
       </c>
       <c r="D44" s="6" t="inlineStr"/>
     </row>
     <row r="45" ht="30.1" customHeight="1">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B45" s="15" t="inlineStr">
         <is>
-          <t>CLINICA DENTAL AMERICA PANAMA        PA</t>
+          <t>ETT*s269ac1RENT        801-8775491   IL</t>
         </is>
       </c>
       <c r="C45" s="7" t="n">
-        <v>-130</v>
+        <v>-369.2</v>
       </c>
       <c r="D45" s="6" t="inlineStr"/>
     </row>
     <row r="46" ht="30.1" customHeight="1">
       <c r="A46" s="4" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>03/05/2021</t>
         </is>
       </c>
       <c r="B46" s="15" t="inlineStr">
         <is>
-          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+          <t>ANTI BURGUER           831-7937      PA</t>
         </is>
       </c>
       <c r="C46" s="7" t="n">
-        <v>-74.34</v>
+        <v>-12</v>
       </c>
       <c r="D46" s="6" t="inlineStr"/>
     </row>
     <row r="47" ht="30.1" customHeight="1">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>04/05/2021</t>
         </is>
       </c>
       <c r="B47" s="15" t="inlineStr">
         <is>
-          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+          <t>Amazon web services    aws.amazon.co WA</t>
         </is>
       </c>
       <c r="C47" s="7" t="n">
-        <v>-121.9</v>
+        <v>-33.21</v>
       </c>
       <c r="D47" s="6" t="inlineStr"/>
     </row>
     <row r="48" ht="30.1" customHeight="1">
       <c r="A48" s="4" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>04/05/2021</t>
         </is>
       </c>
       <c r="B48" s="15" t="inlineStr">
         <is>
-          <t>FELIPE MOTTA</t>
+          <t>Disney Plus            507-8389374   CA</t>
         </is>
       </c>
       <c r="C48" s="7" t="n">
-        <v>-150.83</v>
+        <v>-5.99</v>
       </c>
       <c r="D48" s="6" t="inlineStr"/>
     </row>
     <row r="49" ht="30.1" customHeight="1">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>07/05/2021</t>
         </is>
       </c>
       <c r="B49" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>FARMACIA ARROCHA WESTL PANAMA        PA</t>
         </is>
       </c>
       <c r="C49" s="7" t="n">
-        <v>-74.7</v>
+        <v>-42.04</v>
       </c>
       <c r="D49" s="6" t="inlineStr"/>
     </row>
     <row r="50" ht="30.1" customHeight="1">
       <c r="A50" s="4" t="inlineStr">
         <is>
-          <t>20/04/2021</t>
+          <t>06/05/2021</t>
         </is>
       </c>
       <c r="B50" s="15" t="inlineStr">
         <is>
-          <t>NETFLIX.COM            866-579-7172  CA</t>
+          <t>NOVEY VISTA ALEGRE     PANAMA        PA</t>
         </is>
       </c>
       <c r="C50" s="7" t="n">
-        <v>-15.99</v>
+        <v>-52.42</v>
       </c>
       <c r="D50" s="6" t="inlineStr"/>
     </row>
     <row r="51" ht="30.1" customHeight="1">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>07/05/2021</t>
         </is>
       </c>
       <c r="B51" s="15" t="inlineStr">
         <is>
-          <t>UBER   *EATS           HELP.UBER.COM ON</t>
+          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
         </is>
       </c>
       <c r="C51" s="7" t="n">
-        <v>-2.34</v>
+        <v>-206.98</v>
       </c>
       <c r="D51" s="6" t="inlineStr"/>
     </row>
     <row r="52" ht="30.1" customHeight="1">
       <c r="A52" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>07/05/2021</t>
         </is>
       </c>
       <c r="B52" s="15" t="inlineStr">
         <is>
-          <t>UBER   *EATS           HELP.UBER.COM ON</t>
+          <t>AMZN Mktp CA*2L8WI6VO1 WWW.AMAZON.CA ON</t>
         </is>
       </c>
       <c r="C52" s="7" t="n">
-        <v>-23.37</v>
+        <v>-83.38</v>
       </c>
       <c r="D52" s="6" t="inlineStr"/>
     </row>
     <row r="53" ht="30.1" customHeight="1">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>08/05/2021</t>
         </is>
       </c>
       <c r="B53" s="15" t="inlineStr">
         <is>
-          <t>RIBA SMITH MARKET PLAZ PUERTO CAIMIT PA</t>
+          <t>FARMACIA NUEVO CHORRIL CERRO SILVEST PA</t>
         </is>
       </c>
       <c r="C53" s="7" t="n">
-        <v>-14.75</v>
+        <v>-33.3</v>
       </c>
       <c r="D53" s="6" t="inlineStr"/>
     </row>
     <row r="54" ht="30.1" customHeight="1">
       <c r="A54" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>10/05/2021</t>
         </is>
       </c>
       <c r="B54" s="15" t="inlineStr">
         <is>
-          <t>GONG CHA               PANAMA OESTE  PA</t>
+          <t>RESTAURANTE LUNG FUNG</t>
         </is>
       </c>
       <c r="C54" s="7" t="n">
-        <v>-28.65</v>
+        <v>-59.71</v>
       </c>
       <c r="D54" s="6" t="inlineStr"/>
     </row>
     <row r="55" ht="30.1" customHeight="1">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>19/04/2021</t>
+          <t>12/05/2021</t>
         </is>
       </c>
       <c r="B55" s="15" t="inlineStr">
         <is>
-          <t>PAYPAL *FLOWERSCAIN    4029357733    ON</t>
+          <t>FARMACIA ARROCHA ARRAI PANAMA        PA</t>
         </is>
       </c>
       <c r="C55" s="7" t="n">
-        <v>-87.90000000000001</v>
+        <v>-49.65</v>
       </c>
       <c r="D55" s="6" t="inlineStr"/>
     </row>
     <row r="56" ht="30.1" customHeight="1">
       <c r="A56" s="4" t="inlineStr">
         <is>
-          <t>15/05/2021</t>
+          <t>11/05/2021</t>
         </is>
       </c>
       <c r="B56" s="15" t="inlineStr">
         <is>
-          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+          <t>ESTACION MISTI         PANAMA OESTE  PA</t>
         </is>
       </c>
       <c r="C56" s="7" t="n">
-        <v>-95.26000000000001</v>
+        <v>-37</v>
       </c>
       <c r="D56" s="6" t="inlineStr"/>
     </row>
     <row r="57" ht="30.1" customHeight="1">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>15/05/2021</t>
+          <t>12/05/2021</t>
         </is>
       </c>
       <c r="B57" s="15" t="inlineStr">
         <is>
-          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+          <t>VIAJEMOS.COM           7862359135    FL</t>
         </is>
       </c>
       <c r="C57" s="7" t="n">
-        <v>-187.83</v>
+        <v>-991.15</v>
       </c>
       <c r="D57" s="6" t="inlineStr"/>
     </row>
     <row r="58" ht="30.1" customHeight="1">
       <c r="A58" s="4" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>12/05/2021</t>
         </is>
       </c>
       <c r="B58" s="15" t="inlineStr">
         <is>
-          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+          <t>ESA FLACA RICA</t>
         </is>
       </c>
       <c r="C58" s="7" t="n">
-        <v>-323.08</v>
+        <v>-15.78</v>
       </c>
       <c r="D58" s="6" t="inlineStr"/>
     </row>
     <row r="59" ht="30.1" customHeight="1">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>14/05/2021</t>
+          <t>13/05/2021</t>
         </is>
       </c>
       <c r="B59" s="15" t="inlineStr">
         <is>
-          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C59" s="7" t="n">
-        <v>-485.45</v>
+        <v>-234.99</v>
       </c>
       <c r="D59" s="6" t="inlineStr"/>
     </row>
     <row r="60" ht="30.1" customHeight="1">
       <c r="A60" s="4" t="inlineStr">
         <is>
-          <t>12/05/2021</t>
+          <t>15/05/2021</t>
         </is>
       </c>
       <c r="B60" s="15" t="inlineStr">
         <is>
-          <t>PRICESMART COSTA VERDE PANAMA        PA</t>
+          <t>ESTACION MISTI         PANAMA OESTE  PA</t>
         </is>
       </c>
       <c r="C60" s="7" t="n">
-        <v>-332.11</v>
+        <v>-27</v>
       </c>
       <c r="D60" s="6" t="inlineStr"/>
     </row>
     <row r="61" ht="30.1" customHeight="1">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>10/05/2021</t>
+          <t>15/05/2021</t>
         </is>
       </c>
       <c r="B61" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>DELICIAS DEL MAR REST  RIO HATO      PA</t>
         </is>
       </c>
       <c r="C61" s="7" t="n">
-        <v>-250.48</v>
+        <v>-93.3</v>
       </c>
       <c r="D61" s="6" t="inlineStr"/>
     </row>
     <row r="62" ht="30.1" customHeight="1">
       <c r="A62" s="4" t="inlineStr">
         <is>
-          <t>08/05/2021</t>
+          <t>20/04/2021</t>
         </is>
       </c>
       <c r="B62" s="15" t="inlineStr">
         <is>
-          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
+          <t>GRUPO F &amp; G INT, S. A. BETHANIA      PA</t>
         </is>
       </c>
       <c r="C62" s="7" t="n">
-        <v>-476.26</v>
+        <v>-43.2</v>
       </c>
       <c r="D62" s="6" t="inlineStr"/>
     </row>
     <row r="63" ht="30.1" customHeight="1">
       <c r="A63" s="4" t="inlineStr">
         <is>
-          <t>06/05/2021</t>
+          <t>20/04/2021</t>
         </is>
       </c>
       <c r="B63" s="15" t="inlineStr">
         <is>
-          <t>FELIPE MOTTA</t>
+          <t>CANON PANAMA           BETHANIA      PA</t>
         </is>
       </c>
       <c r="C63" s="7" t="n">
-        <v>-64.95</v>
+        <v>-3500</v>
       </c>
       <c r="D63" s="6" t="inlineStr"/>
     </row>
     <row r="64" ht="30.1" customHeight="1">
       <c r="A64" s="4" t="inlineStr">
         <is>
-          <t>06/05/2021</t>
+          <t>21/04/2021</t>
         </is>
       </c>
       <c r="B64" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
         </is>
       </c>
       <c r="C64" s="7" t="n">
-        <v>-287.32</v>
+        <v>-37.63</v>
       </c>
       <c r="D64" s="6" t="inlineStr"/>
     </row>
     <row r="65" ht="30.1" customHeight="1">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>05/05/2021</t>
+          <t>21/04/2021</t>
         </is>
       </c>
       <c r="B65" s="15" t="inlineStr">
         <is>
-          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
         </is>
       </c>
       <c r="C65" s="7" t="n">
-        <v>-432.41</v>
+        <v>-90.68000000000001</v>
       </c>
       <c r="D65" s="6" t="inlineStr"/>
     </row>
     <row r="66" ht="30.1" customHeight="1">
       <c r="A66" s="4" t="inlineStr">
         <is>
-          <t>04/05/2021</t>
+          <t>22/04/2021</t>
         </is>
       </c>
       <c r="B66" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>TEXACO VISTA ALEGRE    PANAMA        PA</t>
         </is>
       </c>
       <c r="C66" s="7" t="n">
-        <v>-243.34</v>
+        <v>-38</v>
       </c>
       <c r="D66" s="6" t="inlineStr"/>
     </row>
     <row r="67" ht="30.1" customHeight="1">
       <c r="A67" s="4" t="inlineStr">
         <is>
-          <t>29/04/2021</t>
+          <t>22/04/2021</t>
         </is>
       </c>
       <c r="B67" s="15" t="inlineStr">
         <is>
-          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+          <t>RIBA SMITH MARKET PLAZ PUERTO CAIMIT PA</t>
         </is>
       </c>
       <c r="C67" s="7" t="n">
-        <v>-386.5</v>
+        <v>-45.42</v>
       </c>
       <c r="D67" s="6" t="inlineStr"/>
     </row>
     <row r="68" ht="30.1" customHeight="1">
       <c r="A68" s="4" t="inlineStr">
         <is>
-          <t>28/04/2021</t>
+          <t>24/04/2021</t>
         </is>
       </c>
       <c r="B68" s="15" t="inlineStr">
         <is>
-          <t>BOUTIQUE CROCS WESTLAN PANAMA OESTE  PA</t>
+          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
         </is>
       </c>
       <c r="C68" s="7" t="n">
-        <v>-35.26</v>
+        <v>-108.33</v>
       </c>
       <c r="D68" s="6" t="inlineStr"/>
     </row>
@@ -1713,11 +1713,11 @@
       </c>
       <c r="B69" s="15" t="inlineStr">
         <is>
-          <t>GRUPO F &amp; G INT, S. A. BETHANIA      PA</t>
+          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
         </is>
       </c>
       <c r="C69" s="7" t="n">
-        <v>-45</v>
+        <v>-121.31</v>
       </c>
       <c r="D69" s="6" t="inlineStr"/>
     </row>
@@ -1729,131 +1729,250 @@
       </c>
       <c r="B70" s="15" t="inlineStr">
         <is>
-          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
+          <t>GRUPO F &amp; G INT, S. A. BETHANIA      PA</t>
         </is>
       </c>
       <c r="C70" s="7" t="n">
-        <v>-121.31</v>
+        <v>-45</v>
       </c>
       <c r="D70" s="6" t="inlineStr"/>
     </row>
     <row r="71" ht="30.1" customHeight="1">
       <c r="A71" s="4" t="inlineStr">
         <is>
-          <t>24/04/2021</t>
+          <t>28/04/2021</t>
         </is>
       </c>
       <c r="B71" s="15" t="inlineStr">
         <is>
-          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+          <t>BOUTIQUE CROCS WESTLAN PANAMA OESTE  PA</t>
         </is>
       </c>
       <c r="C71" s="7" t="n">
-        <v>-108.33</v>
+        <v>-35.26</v>
       </c>
       <c r="D71" s="6" t="inlineStr"/>
     </row>
     <row r="72" ht="30.1" customHeight="1">
       <c r="A72" s="4" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>29/04/2021</t>
         </is>
       </c>
       <c r="B72" s="15" t="inlineStr">
         <is>
-          <t>TEXACO VISTA ALEGRE    PANAMA        PA</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C72" s="7" t="n">
-        <v>-38</v>
+        <v>-386.5</v>
       </c>
       <c r="D72" s="6" t="inlineStr"/>
     </row>
     <row r="73" ht="30.1" customHeight="1">
       <c r="A73" s="4" t="inlineStr">
         <is>
-          <t>22/04/2021</t>
+          <t>04/05/2021</t>
         </is>
       </c>
       <c r="B73" s="15" t="inlineStr">
         <is>
-          <t>RIBA SMITH MARKET PLAZ PUERTO CAIMIT PA</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C73" s="7" t="n">
-        <v>-45.42</v>
+        <v>-243.34</v>
       </c>
       <c r="D73" s="6" t="inlineStr"/>
     </row>
     <row r="74" ht="30.1" customHeight="1">
       <c r="A74" s="4" t="inlineStr">
         <is>
-          <t>21/04/2021</t>
+          <t>05/05/2021</t>
         </is>
       </c>
       <c r="B74" s="15" t="inlineStr">
         <is>
-          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
+          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
         </is>
       </c>
       <c r="C74" s="7" t="n">
-        <v>-37.63</v>
+        <v>-432.41</v>
       </c>
       <c r="D74" s="6" t="inlineStr"/>
     </row>
     <row r="75" ht="30.1" customHeight="1">
       <c r="A75" s="4" t="inlineStr">
         <is>
-          <t>21/04/2021</t>
+          <t>06/05/2021</t>
         </is>
       </c>
       <c r="B75" s="15" t="inlineStr">
         <is>
-          <t>COCHEZ VISTA ALEGRE    PANAMA        PA</t>
+          <t>FELIPE MOTTA</t>
         </is>
       </c>
       <c r="C75" s="7" t="n">
-        <v>-90.68000000000001</v>
+        <v>-64.95</v>
       </c>
       <c r="D75" s="6" t="inlineStr"/>
     </row>
     <row r="76" ht="30.1" customHeight="1">
       <c r="A76" s="4" t="inlineStr">
         <is>
-          <t>20/04/2021</t>
+          <t>06/05/2021</t>
         </is>
       </c>
       <c r="B76" s="15" t="inlineStr">
         <is>
-          <t>GRUPO F &amp; G INT, S. A. BETHANIA      PA</t>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
         </is>
       </c>
       <c r="C76" s="7" t="n">
-        <v>-43.2</v>
+        <v>-287.32</v>
       </c>
       <c r="D76" s="6" t="inlineStr"/>
     </row>
     <row r="77" ht="30.1" customHeight="1">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>20/04/2021</t>
+          <t>08/05/2021</t>
         </is>
       </c>
       <c r="B77" s="15" t="inlineStr">
         <is>
-          <t>CANON PANAMA           BETHANIA      PA</t>
+          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
         </is>
       </c>
       <c r="C77" s="7" t="n">
-        <v>-3500</v>
+        <v>-476.26</v>
       </c>
       <c r="D77" s="6" t="inlineStr"/>
     </row>
+    <row r="78" ht="30.1" customHeight="1">
+      <c r="A78" s="4" t="inlineStr">
+        <is>
+          <t>10/05/2021</t>
+        </is>
+      </c>
+      <c r="B78" s="15" t="inlineStr">
+        <is>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+        </is>
+      </c>
+      <c r="C78" s="7" t="n">
+        <v>-250.48</v>
+      </c>
+      <c r="D78" s="6" t="inlineStr"/>
+    </row>
+    <row r="79" ht="30.1" customHeight="1">
+      <c r="A79" s="4" t="inlineStr">
+        <is>
+          <t>12/05/2021</t>
+        </is>
+      </c>
+      <c r="B79" s="15" t="inlineStr">
+        <is>
+          <t>PRICESMART COSTA VERDE PANAMA        PA</t>
+        </is>
+      </c>
+      <c r="C79" s="7" t="n">
+        <v>-332.11</v>
+      </c>
+      <c r="D79" s="6" t="inlineStr"/>
+    </row>
+    <row r="80" ht="30.1" customHeight="1">
+      <c r="A80" s="4" t="inlineStr">
+        <is>
+          <t>15/05/2021</t>
+        </is>
+      </c>
+      <c r="B80" s="15" t="inlineStr">
+        <is>
+          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+        </is>
+      </c>
+      <c r="C80" s="7" t="n">
+        <v>-95.26000000000001</v>
+      </c>
+      <c r="D80" s="6" t="inlineStr"/>
+    </row>
+    <row r="81" ht="30.1" customHeight="1">
+      <c r="A81" s="4" t="inlineStr">
+        <is>
+          <t>15/05/2021</t>
+        </is>
+      </c>
+      <c r="B81" s="15" t="inlineStr">
+        <is>
+          <t>PRODUCTOS ALIMENTICIOS PANAMA        PA</t>
+        </is>
+      </c>
+      <c r="C81" s="7" t="n">
+        <v>-187.83</v>
+      </c>
+      <c r="D81" s="6" t="inlineStr"/>
+    </row>
+    <row r="82" ht="30.1" customHeight="1">
+      <c r="A82" s="4" t="inlineStr">
+        <is>
+          <t>14/05/2021</t>
+        </is>
+      </c>
+      <c r="B82" s="15" t="inlineStr">
+        <is>
+          <t>MPOS AGENCIAS FEDURO S BETANIA       PA</t>
+        </is>
+      </c>
+      <c r="C82" s="7" t="n">
+        <v>-323.08</v>
+      </c>
+      <c r="D82" s="6" t="inlineStr"/>
+    </row>
+    <row r="83" ht="30.1" customHeight="1">
+      <c r="A83" s="4" t="inlineStr">
+        <is>
+          <t>14/05/2021</t>
+        </is>
+      </c>
+      <c r="B83" s="15" t="inlineStr">
+        <is>
+          <t>VARELA HERMANOS RUTAS  JUAN DIAZ     PA</t>
+        </is>
+      </c>
+      <c r="C83" s="7" t="n">
+        <v>-485.45</v>
+      </c>
+      <c r="D83" s="6" t="inlineStr"/>
+    </row>
+    <row r="84" ht="30.1" customHeight="1">
+      <c r="A84" s="4" t="inlineStr">
+        <is>
+          <t>17/05/2021</t>
+        </is>
+      </c>
+      <c r="B84" s="15" t="inlineStr">
+        <is>
+          <t>MPOS INDUSTRIAS LACTEA FEUILLET      PA</t>
+        </is>
+      </c>
+      <c r="C84" s="7" t="n">
+        <v>-280.19</v>
+      </c>
+      <c r="D84" s="6" t="inlineStr"/>
+    </row>
   </sheetData>
-  <mergeCells count="73">
+  <mergeCells count="80">
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
     <mergeCell ref="F75:H75"/>
     <mergeCell ref="F76:H76"/>
     <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
     <mergeCell ref="F70:H70"/>
     <mergeCell ref="F71:H71"/>
     <mergeCell ref="F72:H72"/>

</xml_diff>